<commit_message>
Additional input data corrections
</commit_message>
<xml_diff>
--- a/InputData/elec/PTCF/Peak Time Capacity Factors.xlsx
+++ b/InputData/elec/PTCF/Peak Time Capacity Factors.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -1138,25 +1138,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="73.85546875" customWidth="1"/>
-    <col min="5" max="5" width="58.7109375" customWidth="1"/>
-    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.265625" customWidth="1"/>
+    <col min="2" max="2" width="73.86328125" customWidth="1"/>
+    <col min="5" max="5" width="58.73046875" customWidth="1"/>
+    <col min="8" max="8" width="47.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>38</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5" s="3">
         <v>2018</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>37</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B7" s="34" t="s">
         <v>36</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>35</v>
       </c>
@@ -1207,85 +1207,85 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B12" s="3">
         <v>2017</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B14" s="33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -1307,15 +1307,15 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="80" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
@@ -1323,7 +1323,7 @@
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>20</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>3697</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>25</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>10346</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="17" t="s">
         <v>26</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>3262</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="20" t="s">
         <v>27</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="17" t="s">
         <v>28</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="20" t="s">
         <v>29</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>3255</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="17" t="s">
         <v>30</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>3471</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="23" t="s">
         <v>31</v>
       </c>
@@ -1459,22 +1459,22 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.265625" customWidth="1"/>
+    <col min="2" max="2" width="27.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1515,15 +1515,15 @@
         <v>0.25720512122037592</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>0.25720512122037592</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>43</v>
       </c>

</xml_diff>